<commit_message>
gift- finalized the survey spreadsheets!
</commit_message>
<xml_diff>
--- a/Master_Spreadsheet_Border_Project.xlsx
+++ b/Master_Spreadsheet_Border_Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gift/Documents/Rprojects/border_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907FAC57-7300-994D-AB8A-0E865883611C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47C75809-3D5A-4A43-888B-A359A60A8BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="500" windowWidth="28800" windowHeight="15380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2060" yWindow="500" windowWidth="28800" windowHeight="15380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="combined" sheetId="12" r:id="rId1"/>
@@ -3396,7 +3396,7 @@
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -3629,6 +3629,9 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="42" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -23839,7 +23842,7 @@
   <dimension ref="A1:AD38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+      <selection activeCell="AF4" sqref="AF4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -40579,7 +40582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399D1F91-4B6C-BE40-98A7-1EECF5204B44}">
   <dimension ref="A1:X93"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="D2" sqref="D2:D29"/>
     </sheetView>
   </sheetViews>
@@ -56164,7 +56167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B8ED26-E227-7B45-9CF7-C1D2C81BE591}">
   <dimension ref="A1:AG79"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
+    <sheetView zoomScale="151" zoomScaleNormal="151" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -68156,8 +68159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B182E629-28D6-8147-A91B-FFEACEDE4BDD}">
   <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="AA45" sqref="AA45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -69210,16 +69213,16 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="16">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="104" t="s">
         <v>737</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="104" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="85" t="s">
+      <c r="C14" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E14" s="86">
@@ -69290,16 +69293,16 @@
       </c>
     </row>
     <row r="15" spans="1:26" ht="16">
-      <c r="A15" s="32" t="s">
+      <c r="A15" s="104" t="s">
         <v>738</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="104" t="s">
         <v>189</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D15" s="93" t="s">
+      <c r="D15" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E15" s="86">
@@ -69450,16 +69453,16 @@
       </c>
     </row>
     <row r="17" spans="1:26" ht="16">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="104" t="s">
         <v>740</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="104" t="s">
         <v>197</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D17" s="93" t="s">
+      <c r="D17" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E17" s="86">
@@ -69530,16 +69533,16 @@
       </c>
     </row>
     <row r="18" spans="1:26" ht="16">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="104" t="s">
         <v>741</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="104" t="s">
         <v>201</v>
       </c>
-      <c r="C18" s="85" t="s">
+      <c r="C18" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D18" s="93" t="s">
+      <c r="D18" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E18" s="86">
@@ -69610,16 +69613,16 @@
       </c>
     </row>
     <row r="19" spans="1:26" ht="16">
-      <c r="A19" s="32" t="s">
+      <c r="A19" s="104" t="s">
         <v>742</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="104" t="s">
         <v>205</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D19" s="93" t="s">
+      <c r="D19" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E19" s="86">
@@ -69770,16 +69773,16 @@
       </c>
     </row>
     <row r="21" spans="1:26" ht="16">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="104" t="s">
         <v>744</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="104" t="s">
         <v>213</v>
       </c>
-      <c r="C21" s="85" t="s">
+      <c r="C21" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D21" s="93" t="s">
+      <c r="D21" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E21" s="86">
@@ -70417,16 +70420,16 @@
       </c>
     </row>
     <row r="29" spans="1:26" ht="16">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="104" t="s">
         <v>752</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="104" t="s">
         <v>314</v>
       </c>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D29" s="93" t="s">
+      <c r="D29" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E29" s="86">
@@ -70498,16 +70501,16 @@
       </c>
     </row>
     <row r="30" spans="1:26" ht="16">
-      <c r="A30" s="32" t="s">
+      <c r="A30" s="104" t="s">
         <v>753</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="104" t="s">
         <v>318</v>
       </c>
-      <c r="C30" s="85" t="s">
+      <c r="C30" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D30" s="93" t="s">
+      <c r="D30" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E30" s="86">
@@ -70579,16 +70582,16 @@
       </c>
     </row>
     <row r="31" spans="1:26" ht="16">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="104" t="s">
         <v>754</v>
       </c>
-      <c r="B31" s="32" t="s">
+      <c r="B31" s="104" t="s">
         <v>322</v>
       </c>
-      <c r="C31" s="85" t="s">
+      <c r="C31" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D31" s="93" t="s">
+      <c r="D31" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E31" s="86">
@@ -70660,16 +70663,16 @@
       </c>
     </row>
     <row r="32" spans="1:26" ht="16">
-      <c r="A32" s="32" t="s">
+      <c r="A32" s="104" t="s">
         <v>755</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="104" t="s">
         <v>326</v>
       </c>
-      <c r="C32" s="85" t="s">
+      <c r="C32" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D32" s="93" t="s">
+      <c r="D32" s="106" t="s">
         <v>697</v>
       </c>
       <c r="E32" s="86">
@@ -70741,17 +70744,17 @@
       </c>
     </row>
     <row r="33" spans="1:26" ht="16">
-      <c r="A33" s="32" t="s">
+      <c r="A33" s="104" t="s">
         <v>756</v>
       </c>
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="104" t="s">
         <v>330</v>
       </c>
-      <c r="C33" s="85" t="s">
+      <c r="C33" s="105" t="s">
         <v>828</v>
       </c>
-      <c r="D33" s="94" t="s">
-        <v>854</v>
+      <c r="D33" s="106" t="s">
+        <v>697</v>
       </c>
       <c r="E33" s="86">
         <v>10.5899</v>

</xml_diff>